<commit_message>
update the output file
</commit_message>
<xml_diff>
--- a/outputs/germline_VaraintBasedArray.xlsx
+++ b/outputs/germline_VaraintBasedArray.xlsx
@@ -419,12 +419,12 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>{i}</t>
+          <t>germline_test01</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>{i}</t>
+          <t>germline_test02</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -498,7 +498,7 @@
         </is>
       </c>
       <c r="N2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -566,7 +566,7 @@
         </is>
       </c>
       <c r="N3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="N4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="N5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="N6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -838,7 +838,7 @@
         </is>
       </c>
       <c r="N7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -906,7 +906,7 @@
         </is>
       </c>
       <c r="N8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="N9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="N10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="N11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -1178,7 +1178,7 @@
         </is>
       </c>
       <c r="N12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -1246,7 +1246,7 @@
         </is>
       </c>
       <c r="N13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -1314,7 +1314,7 @@
         </is>
       </c>
       <c r="N14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="N15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1450,7 +1450,7 @@
         </is>
       </c>
       <c r="N16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -1518,7 +1518,7 @@
         </is>
       </c>
       <c r="N17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1586,7 +1586,7 @@
         </is>
       </c>
       <c r="N18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1654,7 +1654,7 @@
         </is>
       </c>
       <c r="N19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="N20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1790,7 +1790,7 @@
         </is>
       </c>
       <c r="N21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1858,7 +1858,7 @@
         </is>
       </c>
       <c r="N22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -1926,7 +1926,7 @@
         </is>
       </c>
       <c r="N23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1994,7 +1994,7 @@
         </is>
       </c>
       <c r="N24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="N25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -2130,7 +2130,7 @@
         </is>
       </c>
       <c r="N26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -2198,7 +2198,7 @@
         </is>
       </c>
       <c r="N27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -2266,7 +2266,7 @@
         </is>
       </c>
       <c r="N28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -2334,7 +2334,7 @@
         </is>
       </c>
       <c r="N29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -2402,7 +2402,7 @@
         </is>
       </c>
       <c r="N30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -2470,7 +2470,7 @@
         </is>
       </c>
       <c r="N31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -2538,7 +2538,7 @@
         </is>
       </c>
       <c r="N32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -2606,7 +2606,7 @@
         </is>
       </c>
       <c r="N33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -2674,7 +2674,7 @@
         </is>
       </c>
       <c r="N34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -2742,7 +2742,7 @@
         </is>
       </c>
       <c r="N35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -2810,7 +2810,7 @@
         </is>
       </c>
       <c r="N36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -2878,7 +2878,7 @@
         </is>
       </c>
       <c r="N37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -2946,7 +2946,7 @@
         </is>
       </c>
       <c r="N38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -3014,7 +3014,7 @@
         </is>
       </c>
       <c r="N39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -3082,7 +3082,7 @@
         </is>
       </c>
       <c r="N40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -3150,7 +3150,7 @@
         </is>
       </c>
       <c r="N41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -3218,7 +3218,7 @@
         </is>
       </c>
       <c r="N42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -3286,7 +3286,7 @@
         </is>
       </c>
       <c r="N43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -3354,7 +3354,7 @@
         </is>
       </c>
       <c r="N44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -3422,7 +3422,7 @@
         </is>
       </c>
       <c r="N45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -3490,7 +3490,7 @@
         </is>
       </c>
       <c r="N46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -3558,7 +3558,7 @@
         </is>
       </c>
       <c r="N47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -3626,7 +3626,7 @@
         </is>
       </c>
       <c r="N48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -3694,7 +3694,7 @@
         </is>
       </c>
       <c r="N49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -3762,7 +3762,7 @@
         </is>
       </c>
       <c r="N50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -3830,7 +3830,7 @@
         </is>
       </c>
       <c r="N51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -3898,7 +3898,7 @@
         </is>
       </c>
       <c r="N52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -3966,7 +3966,7 @@
         </is>
       </c>
       <c r="N53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -4034,7 +4034,7 @@
         </is>
       </c>
       <c r="N54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -4102,7 +4102,7 @@
         </is>
       </c>
       <c r="N55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -4170,7 +4170,7 @@
         </is>
       </c>
       <c r="N56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -4238,7 +4238,7 @@
         </is>
       </c>
       <c r="N57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -4306,7 +4306,7 @@
         </is>
       </c>
       <c r="N58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -4374,7 +4374,7 @@
         </is>
       </c>
       <c r="N59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -4442,7 +4442,7 @@
         </is>
       </c>
       <c r="N60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -4510,7 +4510,7 @@
         </is>
       </c>
       <c r="N61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -4578,7 +4578,7 @@
         </is>
       </c>
       <c r="N62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -4646,7 +4646,7 @@
         </is>
       </c>
       <c r="N63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -4714,7 +4714,7 @@
         </is>
       </c>
       <c r="N64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -4782,7 +4782,7 @@
         </is>
       </c>
       <c r="N65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -4850,7 +4850,7 @@
         </is>
       </c>
       <c r="N66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -4918,7 +4918,7 @@
         </is>
       </c>
       <c r="N67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -4986,7 +4986,7 @@
         </is>
       </c>
       <c r="N68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -5054,7 +5054,7 @@
         </is>
       </c>
       <c r="N69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -5122,7 +5122,7 @@
         </is>
       </c>
       <c r="N70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -5190,7 +5190,7 @@
         </is>
       </c>
       <c r="N71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -5258,7 +5258,7 @@
         </is>
       </c>
       <c r="N72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -5326,7 +5326,7 @@
         </is>
       </c>
       <c r="N73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -5394,7 +5394,7 @@
         </is>
       </c>
       <c r="N74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -5462,7 +5462,7 @@
         </is>
       </c>
       <c r="N75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -5530,7 +5530,7 @@
         </is>
       </c>
       <c r="N76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -5598,7 +5598,7 @@
         </is>
       </c>
       <c r="N77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -5666,7 +5666,7 @@
         </is>
       </c>
       <c r="N78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -5734,7 +5734,7 @@
         </is>
       </c>
       <c r="N79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -5802,7 +5802,7 @@
         </is>
       </c>
       <c r="N80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -5870,7 +5870,7 @@
         </is>
       </c>
       <c r="N81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -5938,7 +5938,7 @@
         </is>
       </c>
       <c r="N82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -6006,7 +6006,7 @@
         </is>
       </c>
       <c r="N83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -6074,7 +6074,7 @@
         </is>
       </c>
       <c r="N84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -6142,7 +6142,7 @@
         </is>
       </c>
       <c r="N85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -6210,7 +6210,7 @@
         </is>
       </c>
       <c r="N86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -6278,7 +6278,7 @@
         </is>
       </c>
       <c r="N87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -6346,7 +6346,7 @@
         </is>
       </c>
       <c r="N88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -6414,7 +6414,7 @@
         </is>
       </c>
       <c r="N89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -6482,7 +6482,7 @@
         </is>
       </c>
       <c r="N90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -6550,7 +6550,7 @@
         </is>
       </c>
       <c r="N91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -6618,7 +6618,7 @@
         </is>
       </c>
       <c r="N92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -6686,7 +6686,7 @@
         </is>
       </c>
       <c r="N93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -6754,7 +6754,7 @@
         </is>
       </c>
       <c r="N94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -6822,7 +6822,7 @@
         </is>
       </c>
       <c r="N95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -6890,7 +6890,7 @@
         </is>
       </c>
       <c r="N96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -6958,7 +6958,7 @@
         </is>
       </c>
       <c r="N97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -7026,7 +7026,7 @@
         </is>
       </c>
       <c r="N98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -7094,7 +7094,7 @@
         </is>
       </c>
       <c r="N99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -7162,7 +7162,7 @@
         </is>
       </c>
       <c r="N100" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -7230,7 +7230,7 @@
         </is>
       </c>
       <c r="N101" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -7298,7 +7298,7 @@
         </is>
       </c>
       <c r="N102" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
@@ -7366,7 +7366,7 @@
         </is>
       </c>
       <c r="N103" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -7434,7 +7434,7 @@
         </is>
       </c>
       <c r="N104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -7502,7 +7502,7 @@
         </is>
       </c>
       <c r="N105" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
@@ -7570,7 +7570,7 @@
         </is>
       </c>
       <c r="N106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -7638,7 +7638,7 @@
         </is>
       </c>
       <c r="N107" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
@@ -7706,7 +7706,7 @@
         </is>
       </c>
       <c r="N108" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -7774,7 +7774,7 @@
         </is>
       </c>
       <c r="N109" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -7842,7 +7842,7 @@
         </is>
       </c>
       <c r="N110" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
@@ -7910,7 +7910,7 @@
         </is>
       </c>
       <c r="N111" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -7978,7 +7978,7 @@
         </is>
       </c>
       <c r="N112" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
@@ -8046,7 +8046,7 @@
         </is>
       </c>
       <c r="N113" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -8114,7 +8114,7 @@
         </is>
       </c>
       <c r="N114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
@@ -8182,7 +8182,7 @@
         </is>
       </c>
       <c r="N115" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -8250,7 +8250,7 @@
         </is>
       </c>
       <c r="N116" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -8318,7 +8318,7 @@
         </is>
       </c>
       <c r="N117" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118">
@@ -8386,7 +8386,7 @@
         </is>
       </c>
       <c r="N118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -8454,7 +8454,7 @@
         </is>
       </c>
       <c r="N119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -8522,7 +8522,7 @@
         </is>
       </c>
       <c r="N120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -8590,7 +8590,7 @@
         </is>
       </c>
       <c r="N121" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
@@ -8658,7 +8658,7 @@
         </is>
       </c>
       <c r="N122" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123">
@@ -8726,7 +8726,7 @@
         </is>
       </c>
       <c r="N123" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124">
@@ -8794,7 +8794,7 @@
         </is>
       </c>
       <c r="N124" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
@@ -8862,7 +8862,7 @@
         </is>
       </c>
       <c r="N125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
@@ -8930,7 +8930,7 @@
         </is>
       </c>
       <c r="N126" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
@@ -8998,7 +8998,7 @@
         </is>
       </c>
       <c r="N127" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128">
@@ -9066,7 +9066,7 @@
         </is>
       </c>
       <c r="N128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
@@ -9134,7 +9134,7 @@
         </is>
       </c>
       <c r="N129" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130">
@@ -9202,7 +9202,7 @@
         </is>
       </c>
       <c r="N130" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
@@ -9270,7 +9270,7 @@
         </is>
       </c>
       <c r="N131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -9338,7 +9338,7 @@
         </is>
       </c>
       <c r="N132" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133">
@@ -9406,7 +9406,7 @@
         </is>
       </c>
       <c r="N133" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
@@ -9474,7 +9474,7 @@
         </is>
       </c>
       <c r="N134" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
@@ -9542,7 +9542,7 @@
         </is>
       </c>
       <c r="N135" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
@@ -9610,7 +9610,7 @@
         </is>
       </c>
       <c r="N136" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
@@ -9678,7 +9678,7 @@
         </is>
       </c>
       <c r="N137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
@@ -9746,7 +9746,7 @@
         </is>
       </c>
       <c r="N138" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
@@ -9814,7 +9814,7 @@
         </is>
       </c>
       <c r="N139" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
@@ -9882,7 +9882,7 @@
         </is>
       </c>
       <c r="N140" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
@@ -9950,7 +9950,7 @@
         </is>
       </c>
       <c r="N141" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142">
@@ -10018,7 +10018,7 @@
         </is>
       </c>
       <c r="N142" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
@@ -10086,7 +10086,7 @@
         </is>
       </c>
       <c r="N143" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -10154,7 +10154,7 @@
         </is>
       </c>
       <c r="N144" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
@@ -10222,7 +10222,7 @@
         </is>
       </c>
       <c r="N145" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146">
@@ -10290,7 +10290,7 @@
         </is>
       </c>
       <c r="N146" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
@@ -10358,7 +10358,7 @@
         </is>
       </c>
       <c r="N147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
@@ -10426,7 +10426,7 @@
         </is>
       </c>
       <c r="N148" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -10494,7 +10494,7 @@
         </is>
       </c>
       <c r="N149" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
@@ -10562,7 +10562,7 @@
         </is>
       </c>
       <c r="N150" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
@@ -10630,7 +10630,7 @@
         </is>
       </c>
       <c r="N151" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152">
@@ -10698,7 +10698,7 @@
         </is>
       </c>
       <c r="N152" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153">
@@ -10766,7 +10766,7 @@
         </is>
       </c>
       <c r="N153" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154">
@@ -10834,7 +10834,7 @@
         </is>
       </c>
       <c r="N154" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">
@@ -10902,7 +10902,7 @@
         </is>
       </c>
       <c r="N155" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156">
@@ -10970,7 +10970,7 @@
         </is>
       </c>
       <c r="N156" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -11038,7 +11038,7 @@
         </is>
       </c>
       <c r="N157" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158">
@@ -11106,7 +11106,7 @@
         </is>
       </c>
       <c r="N158" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -11174,7 +11174,7 @@
         </is>
       </c>
       <c r="N159" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
@@ -11242,7 +11242,7 @@
         </is>
       </c>
       <c r="N160" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -11310,7 +11310,7 @@
         </is>
       </c>
       <c r="N161" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162">
@@ -11378,7 +11378,7 @@
         </is>
       </c>
       <c r="N162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
@@ -11446,7 +11446,7 @@
         </is>
       </c>
       <c r="N163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -11514,7 +11514,7 @@
         </is>
       </c>
       <c r="N164" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -11582,7 +11582,7 @@
         </is>
       </c>
       <c r="N165" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166">
@@ -11650,7 +11650,7 @@
         </is>
       </c>
       <c r="N166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167">
@@ -11718,7 +11718,7 @@
         </is>
       </c>
       <c r="N167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -11786,7 +11786,7 @@
         </is>
       </c>
       <c r="N168" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -11854,7 +11854,7 @@
         </is>
       </c>
       <c r="N169" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
@@ -11922,7 +11922,7 @@
         </is>
       </c>
       <c r="N170" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171">
@@ -11990,7 +11990,7 @@
         </is>
       </c>
       <c r="N171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
@@ -12058,7 +12058,7 @@
         </is>
       </c>
       <c r="N172" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
@@ -12126,7 +12126,7 @@
         </is>
       </c>
       <c r="N173" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174">
@@ -12194,7 +12194,7 @@
         </is>
       </c>
       <c r="N174" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175">
@@ -12262,7 +12262,7 @@
         </is>
       </c>
       <c r="N175" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176">
@@ -12330,7 +12330,7 @@
         </is>
       </c>
       <c r="N176" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -12398,7 +12398,7 @@
         </is>
       </c>
       <c r="N177" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178">
@@ -12466,7 +12466,7 @@
         </is>
       </c>
       <c r="N178" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179">
@@ -12534,7 +12534,7 @@
         </is>
       </c>
       <c r="N179" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180">
@@ -12602,7 +12602,7 @@
         </is>
       </c>
       <c r="N180" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181">
@@ -12670,7 +12670,7 @@
         </is>
       </c>
       <c r="N181" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
@@ -12738,7 +12738,7 @@
         </is>
       </c>
       <c r="N182" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183">
@@ -12806,7 +12806,7 @@
         </is>
       </c>
       <c r="N183" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184">
@@ -12874,7 +12874,7 @@
         </is>
       </c>
       <c r="N184" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">
@@ -12942,7 +12942,7 @@
         </is>
       </c>
       <c r="N185" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
@@ -13010,7 +13010,7 @@
         </is>
       </c>
       <c r="N186" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -13078,7 +13078,7 @@
         </is>
       </c>
       <c r="N187" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188">
@@ -13146,7 +13146,7 @@
         </is>
       </c>
       <c r="N188" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189">
@@ -13214,7 +13214,7 @@
         </is>
       </c>
       <c r="N189" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">
@@ -13282,7 +13282,7 @@
         </is>
       </c>
       <c r="N190" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">
@@ -13350,7 +13350,7 @@
         </is>
       </c>
       <c r="N191" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192">
@@ -13418,7 +13418,7 @@
         </is>
       </c>
       <c r="N192" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193">
@@ -13486,7 +13486,7 @@
         </is>
       </c>
       <c r="N193" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
@@ -13554,7 +13554,7 @@
         </is>
       </c>
       <c r="N194" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195">
@@ -13622,7 +13622,7 @@
         </is>
       </c>
       <c r="N195" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">
@@ -13690,7 +13690,7 @@
         </is>
       </c>
       <c r="N196" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197">
@@ -13758,7 +13758,7 @@
         </is>
       </c>
       <c r="N197" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198">
@@ -13826,7 +13826,7 @@
         </is>
       </c>
       <c r="N198" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199">
@@ -13894,7 +13894,7 @@
         </is>
       </c>
       <c r="N199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -13962,7 +13962,7 @@
         </is>
       </c>
       <c r="N200" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201">
@@ -14030,7 +14030,7 @@
         </is>
       </c>
       <c r="N201" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202">
@@ -14098,7 +14098,7 @@
         </is>
       </c>
       <c r="N202" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203">
@@ -14166,7 +14166,7 @@
         </is>
       </c>
       <c r="N203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204">
@@ -14234,7 +14234,7 @@
         </is>
       </c>
       <c r="N204" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205">
@@ -14302,7 +14302,7 @@
         </is>
       </c>
       <c r="N205" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206">
@@ -14370,7 +14370,7 @@
         </is>
       </c>
       <c r="N206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207">
@@ -14438,7 +14438,7 @@
         </is>
       </c>
       <c r="N207" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208">
@@ -14506,7 +14506,7 @@
         </is>
       </c>
       <c r="N208" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209">
@@ -14574,7 +14574,7 @@
         </is>
       </c>
       <c r="N209" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210">
@@ -14642,7 +14642,7 @@
         </is>
       </c>
       <c r="N210" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211">
@@ -14710,7 +14710,7 @@
         </is>
       </c>
       <c r="N211" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212">
@@ -14778,7 +14778,7 @@
         </is>
       </c>
       <c r="N212" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213">
@@ -14846,7 +14846,7 @@
         </is>
       </c>
       <c r="N213" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214">
@@ -14914,7 +14914,7 @@
         </is>
       </c>
       <c r="N214" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215">
@@ -14982,7 +14982,7 @@
         </is>
       </c>
       <c r="N215" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216">
@@ -15050,7 +15050,7 @@
         </is>
       </c>
       <c r="N216" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217">
@@ -15118,7 +15118,7 @@
         </is>
       </c>
       <c r="N217" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218">
@@ -15186,7 +15186,7 @@
         </is>
       </c>
       <c r="N218" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219">
@@ -15254,7 +15254,7 @@
         </is>
       </c>
       <c r="N219" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220">
@@ -15322,7 +15322,7 @@
         </is>
       </c>
       <c r="N220" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221">
@@ -15390,7 +15390,7 @@
         </is>
       </c>
       <c r="N221" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222">
@@ -15458,7 +15458,7 @@
         </is>
       </c>
       <c r="N222" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="223">
@@ -15526,7 +15526,7 @@
         </is>
       </c>
       <c r="N223" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224">
@@ -15594,7 +15594,7 @@
         </is>
       </c>
       <c r="N224" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225">
@@ -15662,7 +15662,7 @@
         </is>
       </c>
       <c r="N225" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="226">
@@ -15730,7 +15730,7 @@
         </is>
       </c>
       <c r="N226" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227">
@@ -15798,7 +15798,7 @@
         </is>
       </c>
       <c r="N227" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228">
@@ -15866,7 +15866,7 @@
         </is>
       </c>
       <c r="N228" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229">
@@ -15934,7 +15934,7 @@
         </is>
       </c>
       <c r="N229" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230">
@@ -16002,7 +16002,7 @@
         </is>
       </c>
       <c r="N230" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231">
@@ -16070,7 +16070,7 @@
         </is>
       </c>
       <c r="N231" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="232">
@@ -16138,7 +16138,7 @@
         </is>
       </c>
       <c r="N232" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233">
@@ -16206,7 +16206,7 @@
         </is>
       </c>
       <c r="N233" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="234">
@@ -16274,7 +16274,7 @@
         </is>
       </c>
       <c r="N234" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="235">
@@ -16342,7 +16342,7 @@
         </is>
       </c>
       <c r="N235" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="236">
@@ -16410,7 +16410,7 @@
         </is>
       </c>
       <c r="N236" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237">
@@ -16478,7 +16478,7 @@
         </is>
       </c>
       <c r="N237" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238">
@@ -16546,7 +16546,7 @@
         </is>
       </c>
       <c r="N238" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="239">
@@ -16614,7 +16614,7 @@
         </is>
       </c>
       <c r="N239" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240">
@@ -16682,7 +16682,7 @@
         </is>
       </c>
       <c r="N240" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241">
@@ -16750,7 +16750,7 @@
         </is>
       </c>
       <c r="N241" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242">
@@ -16818,7 +16818,7 @@
         </is>
       </c>
       <c r="N242" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243">
@@ -16886,7 +16886,7 @@
         </is>
       </c>
       <c r="N243" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="244">
@@ -16954,7 +16954,7 @@
         </is>
       </c>
       <c r="N244" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>